<commit_message>
update Project Sample Data.xlsx and initial code for models.py
</commit_message>
<xml_diff>
--- a/assets/Project Sample Data.xlsx
+++ b/assets/Project Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/student/Desktop/Phase-5-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2F8551-66FC-FE40-AF99-C6D84250F97C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E687D5-F34E-FD4F-A525-9C47C4B38010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="7720" windowWidth="23160" windowHeight="16680" activeTab="5" xr2:uid="{32EFB3F7-074C-4947-9292-1B2AC616E0B4}"/>
+    <workbookView xWindow="800" yWindow="5080" windowWidth="28740" windowHeight="14660" activeTab="5" xr2:uid="{32EFB3F7-074C-4947-9292-1B2AC616E0B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Location" sheetId="6" r:id="rId3"/>
     <sheet name="House" sheetId="4" r:id="rId4"/>
     <sheet name="Flight" sheetId="5" r:id="rId5"/>
-    <sheet name="Variables" sheetId="7" r:id="rId6"/>
+    <sheet name="Aircraft" sheetId="8" r:id="rId6"/>
+    <sheet name="Variables" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="231">
   <si>
     <t>User</t>
   </si>
@@ -217,9 +218,6 @@
     <t>Distance</t>
   </si>
   <si>
-    <t>Class</t>
-  </si>
-  <si>
     <t>Destination</t>
   </si>
   <si>
@@ -241,12 +239,6 @@
     <t>OUTPUT</t>
   </si>
   <si>
-    <t>DL 298</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
     <t>{'user ID': 8, 'air carrier/flight number': 'BA 234', 'destination': 'Phoenix', 'class': 'comfort', 'aircraft type': 'Boeing 787', 'CO2 per mile per traveler': 0.20, 'distance (miles)': 500}</t>
   </si>
   <si>
@@ -295,48 +287,9 @@
     <t>{'user ID': 10, 'air carrier/flight number': 'BA 789', 'destination': 'Washington', 'class': 'first class', 'aircraft type': 'Boeing 787', 'CO2 per mile per traveler': 0.28, 'distance (miles)': 1700}</t>
   </si>
   <si>
-    <t>economy</t>
-  </si>
-  <si>
     <t>Aircraft</t>
   </si>
   <si>
-    <t>Boeing 737</t>
-  </si>
-  <si>
-    <t>AA 456</t>
-  </si>
-  <si>
-    <t>Los Angeles</t>
-  </si>
-  <si>
-    <t>comfort</t>
-  </si>
-  <si>
-    <t>Airbus A320</t>
-  </si>
-  <si>
-    <t>UA 123</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>first class</t>
-  </si>
-  <si>
-    <t>Boeing 777</t>
-  </si>
-  <si>
-    <t>SW 789</t>
-  </si>
-  <si>
-    <t>Houston</t>
-  </si>
-  <si>
-    <t>Airbus A380</t>
-  </si>
-  <si>
     <t>Model: Location</t>
   </si>
   <si>
@@ -634,9 +587,6 @@
     <t>Aircraft.name</t>
   </si>
   <si>
-    <t>Aircraft.type</t>
-  </si>
-  <si>
     <t>Flight.co2perMile</t>
   </si>
   <si>
@@ -647,6 +597,288 @@
   </si>
   <si>
     <t>Boolean</t>
+  </si>
+  <si>
+    <t>Departure</t>
+  </si>
+  <si>
+    <t>Model: Aircraft</t>
+  </si>
+  <si>
+    <t>international</t>
+  </si>
+  <si>
+    <t>Seats</t>
+  </si>
+  <si>
+    <t>CO2 per mile and passenger</t>
+  </si>
+  <si>
+    <t>Seattle</t>
+  </si>
+  <si>
+    <t>DL 699</t>
+  </si>
+  <si>
+    <t>Departure Code</t>
+  </si>
+  <si>
+    <t>Destination Code</t>
+  </si>
+  <si>
+    <t>JFK</t>
+  </si>
+  <si>
+    <t>SEA</t>
+  </si>
+  <si>
+    <t>AA 73</t>
+  </si>
+  <si>
+    <t>LAX</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>SYD</t>
+  </si>
+  <si>
+    <t>Boeing 777-300ER</t>
+  </si>
+  <si>
+    <t>Airbus A321neo</t>
+  </si>
+  <si>
+    <t>ORD</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>LHR</t>
+  </si>
+  <si>
+    <t>UA 929</t>
+  </si>
+  <si>
+    <t>Boeing 767-300</t>
+  </si>
+  <si>
+    <t>INTERM,</t>
+  </si>
+  <si>
+    <t>DL 2172</t>
+  </si>
+  <si>
+    <t>IAH</t>
+  </si>
+  <si>
+    <t>Detroit</t>
+  </si>
+  <si>
+    <t>DTW</t>
+  </si>
+  <si>
+    <t>Airbus A319</t>
+  </si>
+  <si>
+    <r>
+      <t>Airbus A321neo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Approximately 206-244 seats, depending on the configuration.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Boeing 777-300ER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Typically around 368-451 seats, depending on the airline's configuration.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Boeing 767-300</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Generally around 180-260 seats, depending on the layout.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Airbus A319</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Usually has around 140-160 seats.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Airbus A321neo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Approximately 0.4 to 0.5 gallons per mile.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Boeing 777-300ER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Around 0.5 to 0.6 gallons per mile.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Boeing 767-300</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Typically about 0.4 to 0.5 gallons per mile.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Airbus A319</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Roughly 0.3 to 0.4 gallons per mile.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Airbus A321neo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Approximately 80-100 grams of CO2 per seat per mile.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Boeing 777-300ER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Roughly 90-110 grams of CO2 per seat per mile.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Boeing 767-300</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: About 70-90 grams of CO2 per seat per mile.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Airbus A319</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Approximately 70-90 grams of CO2 per seat per mile.</t>
+    </r>
+  </si>
+  <si>
+    <t>Gallons</t>
+  </si>
+  <si>
+    <t>for distance (return trip)</t>
+  </si>
+  <si>
+    <t>kg CO2</t>
+  </si>
+  <si>
+    <t>gallons per (100 passenger miles)</t>
+  </si>
+  <si>
+    <t>g CO3 per mile and pass</t>
+  </si>
+  <si>
+    <t>CO2 per Trip and pass</t>
   </si>
 </sst>
 </file>
@@ -657,7 +889,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -706,8 +938,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -729,6 +969,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -764,7 +1010,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -878,24 +1124,35 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1292,10 +1549,10 @@
         <v>9</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
@@ -1323,7 +1580,7 @@
         <v>56</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>11</v>
@@ -1337,13 +1594,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>56</v>
@@ -1354,7 +1611,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>10</v>
@@ -1443,7 +1700,7 @@
   <dimension ref="B2:F28"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F5" sqref="F5:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1703,7 +1960,7 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1728,19 +1985,19 @@
         <v>20</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
@@ -1766,7 +2023,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
@@ -1978,7 +2235,7 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="D16" s="3">
         <v>0.18340000000000001</v>
@@ -1992,22 +2249,22 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="26" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="27" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="27" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="27" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2024,7 +2281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE410F25-C2D1-0E47-B65D-2476561BC1C2}">
   <dimension ref="B2:L21"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="125" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -2045,7 +2302,7 @@
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="K2" s="1"/>
     </row>
@@ -2059,13 +2316,13 @@
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="22" t="s">
         <v>64</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="K3" s="22" t="s">
-        <v>65</v>
       </c>
       <c r="L3" s="20"/>
     </row>
@@ -2074,16 +2331,16 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>20</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>44</v>
@@ -2095,7 +2352,7 @@
         <v>53</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="K4" s="21" t="s">
         <v>54</v>
@@ -2504,7 +2761,7 @@
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
       <c r="D16" s="2" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="E16" s="28">
         <f>MIN(E5:E14)</f>
@@ -2535,7 +2792,7 @@
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D17" s="2" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="E17" s="28">
         <f>AVERAGE(E5:E14)</f>
@@ -2564,7 +2821,7 @@
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D18" s="2" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="E18" s="28">
         <f>MAX(E5:E14)</f>
@@ -2601,12 +2858,12 @@
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="32" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2622,14 +2879,18 @@
   <dimension ref="B2:U50"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
-    <col min="3" max="8" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="10.83203125" style="2"/>
+    <col min="4" max="5" width="14.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="2"/>
     <col min="9" max="10" width="13.83203125" style="2" customWidth="1"/>
     <col min="11" max="11" width="10.83203125" style="2"/>
     <col min="12" max="12" width="15.1640625" style="2" customWidth="1"/>
@@ -2646,7 +2907,7 @@
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2660,18 +2921,20 @@
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C3" s="11"/>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="15" t="s">
-        <v>63</v>
+      <c r="G3" s="12"/>
+      <c r="H3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" s="54" t="s">
+        <v>207</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.2">
@@ -2679,31 +2942,31 @@
         <v>12</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="D4" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="J4" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -2721,32 +2984,32 @@
         <v>1</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>66</v>
+        <v>191</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>84</v>
+        <v>194</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="G5" s="17">
+        <v>190</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="H5" s="19">
+        <v>2414</v>
+      </c>
+      <c r="I5" s="53">
         <v>0.35</v>
       </c>
-      <c r="H5" s="17">
-        <v>1500</v>
-      </c>
-      <c r="I5" s="19">
-        <v>0.35</v>
-      </c>
       <c r="J5" s="24">
-        <f>H5*G5</f>
-        <v>525</v>
+        <f>Aircraft!K5</f>
+        <v>217.25999999999996</v>
       </c>
       <c r="K5" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.2">
@@ -2754,32 +3017,32 @@
         <v>2</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>87</v>
+        <v>196</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>89</v>
+        <v>197</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="G6" s="17">
+        <v>198</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="H6" s="19">
+        <v>7494</v>
+      </c>
+      <c r="I6" s="53">
         <v>0.25</v>
       </c>
-      <c r="H6" s="17">
-        <v>2300</v>
-      </c>
-      <c r="I6" s="19">
-        <v>0.25</v>
-      </c>
       <c r="J6" s="24">
-        <f>H6*G6</f>
-        <v>575</v>
+        <f>Aircraft!K6</f>
+        <v>824.34000000000015</v>
       </c>
       <c r="K6" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.2">
@@ -2787,32 +3050,32 @@
         <v>3</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>91</v>
+        <v>205</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>92</v>
+        <v>26</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>93</v>
+        <v>202</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="G7" s="17">
+        <v>203</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="H7" s="19">
+        <v>3942</v>
+      </c>
+      <c r="I7" s="53">
         <v>0.4</v>
       </c>
-      <c r="H7" s="17">
-        <v>800</v>
-      </c>
-      <c r="I7" s="19">
-        <v>0.4</v>
-      </c>
       <c r="J7" s="24">
-        <f>H7*G7</f>
-        <v>320</v>
+        <f>Aircraft!K7</f>
+        <v>354.78000000000003</v>
       </c>
       <c r="K7" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.2">
@@ -2820,254 +3083,265 @@
         <v>4</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>95</v>
+        <v>208</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>84</v>
+        <v>209</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="G8" s="17">
+        <v>210</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="H8" s="19">
+        <v>1075</v>
+      </c>
+      <c r="I8" s="53">
         <v>0.3</v>
       </c>
-      <c r="H8" s="17">
-        <v>1200</v>
-      </c>
-      <c r="I8" s="19">
-        <v>0.3</v>
-      </c>
       <c r="J8" s="24">
-        <f>H8*G8</f>
-        <v>360</v>
+        <f>Aircraft!K8</f>
+        <v>75.25</v>
       </c>
       <c r="K8" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B9" s="3">
         <v>5</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="3"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="44"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>6</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="3"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="44"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <v>7</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="3"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="44"/>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <v>8</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="3"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="44"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <v>9</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="3"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="44"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
         <v>10</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="3"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="44"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <v>11</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="20"/>
+      <c r="C15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <v>12</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="20"/>
+      <c r="C16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="44"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="3">
         <v>13</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="20"/>
+      <c r="C17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="44"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="3">
         <v>14</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="20"/>
-      <c r="L18" s="9"/>
+      <c r="C18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="48"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <v>15</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="20"/>
-      <c r="L19" s="6"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="44"/>
+      <c r="L19" s="49"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
         <v>16</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="20"/>
-      <c r="L20" s="6"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="49"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="3">
         <v>17</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="20"/>
-      <c r="L21" s="6"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="49"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="3">
         <v>18</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="20"/>
-      <c r="L22" s="6"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="49"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="3">
         <v>19</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="20"/>
-      <c r="L23" s="6"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="49"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="3">
         <v>20</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="20"/>
-      <c r="L24" s="6"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="49"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="L25" s="6"/>
@@ -3083,103 +3357,147 @@
     </row>
     <row r="29" spans="2:12" ht="18" x14ac:dyDescent="0.2">
       <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C32" s="25"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C33" s="25"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C34" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C35" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C36" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C37" s="25" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C35" s="25" t="s">
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C38" s="25" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C36" s="25" t="s">
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C39" s="25" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C37" s="25" t="s">
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C40" s="25" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C38" s="25" t="s">
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C41" s="25" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C39" s="25" t="s">
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C42" s="25" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C40" s="25" t="s">
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C43" s="25" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C41" s="25" t="s">
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C44" s="25" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C42" s="25" t="s">
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C45" s="25" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C43" s="25" t="s">
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C46" s="25" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C44" s="25" t="s">
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C47" s="25" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C45" s="25" t="s">
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C48" s="25" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C46" s="25" t="s">
+      <c r="D48" s="25"/>
+      <c r="E48" s="25"/>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C49" s="25" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C47" s="25" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C48" s="25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C49" s="25" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="50" spans="3:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+    </row>
+    <row r="50" spans="3:5" ht="18" x14ac:dyDescent="0.2">
       <c r="C50" s="7" t="s">
         <v>43</v>
       </c>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3187,11 +3505,664 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247AF918-C098-5746-A618-04E4B77230F3}">
+  <dimension ref="B1:U50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="2"/>
+    <col min="6" max="6" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="17.1640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="24.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="2"/>
+    <col min="12" max="12" width="15.1640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15.5" style="2" customWidth="1"/>
+    <col min="14" max="15" width="13.5" style="2" customWidth="1"/>
+    <col min="16" max="16" width="14" style="2" customWidth="1"/>
+    <col min="17" max="17" width="15" style="2" customWidth="1"/>
+    <col min="18" max="18" width="13.1640625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="14.33203125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="15.6640625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="13.1640625" style="2" customWidth="1"/>
+    <col min="22" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+    </row>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="44"/>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C3" s="44"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>187</v>
+      </c>
+      <c r="E4" s="46" t="s">
+        <v>188</v>
+      </c>
+      <c r="F4" s="46" t="s">
+        <v>228</v>
+      </c>
+      <c r="G4" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="H4" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="I4" s="46" t="s">
+        <v>229</v>
+      </c>
+      <c r="J4" s="46" t="s">
+        <v>189</v>
+      </c>
+      <c r="K4" s="46" t="s">
+        <v>230</v>
+      </c>
+      <c r="L4" s="45"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>201</v>
+      </c>
+      <c r="D5" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>225</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G5" s="2">
+        <f>F5*Flight!H5*2*(E5/100)</f>
+        <v>4888.3499999999995</v>
+      </c>
+      <c r="H5" s="2">
+        <f>G5*10</f>
+        <v>48883.499999999993</v>
+      </c>
+      <c r="I5" s="2">
+        <f>H5/E5/G5*1000</f>
+        <v>44.444444444444436</v>
+      </c>
+      <c r="J5" s="47">
+        <v>90</v>
+      </c>
+      <c r="K5" s="47">
+        <f>H5/E5</f>
+        <v>217.25999999999996</v>
+      </c>
+      <c r="L5" s="44"/>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="D6" s="47" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>370</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G6" s="2">
+        <f>F6*Flight!H6*2*(E6/100)</f>
+        <v>30500.580000000005</v>
+      </c>
+      <c r="H6" s="2">
+        <f>G6*10</f>
+        <v>305005.80000000005</v>
+      </c>
+      <c r="I6" s="2">
+        <f>H6/E6/G6*1000</f>
+        <v>27.027027027027028</v>
+      </c>
+      <c r="J6" s="47">
+        <v>100</v>
+      </c>
+      <c r="K6" s="47">
+        <f>H6/E6</f>
+        <v>824.34000000000015</v>
+      </c>
+      <c r="L6" s="44"/>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B7" s="3">
+        <v>3</v>
+      </c>
+      <c r="C7" s="47" t="s">
+        <v>206</v>
+      </c>
+      <c r="D7" s="47" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>220</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G7" s="2">
+        <f>F7*Flight!H7*2*(E7/100)</f>
+        <v>7805.1600000000008</v>
+      </c>
+      <c r="H7" s="2">
+        <f>G7*10</f>
+        <v>78051.600000000006</v>
+      </c>
+      <c r="I7" s="2">
+        <f>H7/E7/G7*1000</f>
+        <v>45.454545454545453</v>
+      </c>
+      <c r="J7" s="47">
+        <v>80</v>
+      </c>
+      <c r="K7" s="47">
+        <f>H7/E7</f>
+        <v>354.78000000000003</v>
+      </c>
+      <c r="L7" s="44"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B8" s="3">
+        <v>4</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="D8" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>150</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="G8" s="2">
+        <f>F8*Flight!H8*2*(E8/100)</f>
+        <v>1128.75</v>
+      </c>
+      <c r="H8" s="2">
+        <f>G8*10</f>
+        <v>11287.5</v>
+      </c>
+      <c r="I8" s="2">
+        <f>H8/E8/G8*1000</f>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="J8" s="47">
+        <v>80</v>
+      </c>
+      <c r="K8" s="47">
+        <f>H8/E8</f>
+        <v>75.25</v>
+      </c>
+      <c r="L8" s="44"/>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B9" s="3">
+        <v>5</v>
+      </c>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="44"/>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B10" s="3"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="44"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B11" s="3"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="44"/>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B12" s="3"/>
+      <c r="C12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="44"/>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B13" s="3"/>
+      <c r="C13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="44"/>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B14" s="3"/>
+      <c r="C14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="44"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B16" s="3"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="44"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B17" s="55" t="s">
+        <v>213</v>
+      </c>
+      <c r="C17" s="47"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="44"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B18" s="55" t="s">
+        <v>214</v>
+      </c>
+      <c r="C18" s="47"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="48"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B19" s="55" t="s">
+        <v>215</v>
+      </c>
+      <c r="C19" s="47"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="44"/>
+      <c r="L19" s="49"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B20" s="55" t="s">
+        <v>216</v>
+      </c>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="49"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B21" s="3"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="49"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B22" s="55" t="s">
+        <v>217</v>
+      </c>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="49"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B23" s="55" t="s">
+        <v>218</v>
+      </c>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="49"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B24" s="55" t="s">
+        <v>219</v>
+      </c>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="49"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B25" s="55" t="s">
+        <v>220</v>
+      </c>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="49"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="49"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B27" s="55" t="s">
+        <v>221</v>
+      </c>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="49"/>
+    </row>
+    <row r="28" spans="2:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="B28" s="55" t="s">
+        <v>222</v>
+      </c>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="50"/>
+    </row>
+    <row r="29" spans="2:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="B29" s="55" t="s">
+        <v>223</v>
+      </c>
+      <c r="C29" s="50"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="44"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B30" s="55" t="s">
+        <v>224</v>
+      </c>
+      <c r="C30" s="51"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="44"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C31" s="25"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C32" s="25"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="25"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C34" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C35" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C36" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C37" s="25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C38" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C39" s="25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C40" s="25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C41" s="25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C42" s="25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C43" s="25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C44" s="25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C45" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C46" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C47" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C48" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C49" s="25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="C50" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47C0C0F9-708C-F34C-ABB4-7A88469AE5BB}">
-  <dimension ref="B2:I37"/>
+  <dimension ref="B2:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3206,7 +4177,7 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
@@ -3230,22 +4201,22 @@
         <v>2</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="G4" s="37" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="H4" s="37" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="I4" s="37" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
@@ -3256,19 +4227,19 @@
         <v>0</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="I5" s="35"/>
     </row>
@@ -3280,22 +4251,22 @@
         <v>0</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="E6" s="38" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="G6" s="38" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="H6" s="38" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="I6" s="40" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
@@ -3306,22 +4277,22 @@
         <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="I7" s="36" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
@@ -3332,19 +4303,19 @@
         <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="I8" s="35"/>
     </row>
@@ -3356,19 +4327,19 @@
         <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="I9" s="35"/>
     </row>
@@ -3380,19 +4351,19 @@
         <v>15</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="E10" s="39" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="F10" s="39" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="G10" s="39" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="H10" s="38" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="I10" s="41"/>
     </row>
@@ -3404,22 +4375,22 @@
         <v>24</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="E11" s="34" t="s">
         <v>8</v>
       </c>
       <c r="F11" s="34" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="H11" s="34" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="I11" s="35" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
@@ -3430,22 +4401,22 @@
         <v>24</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="E12" s="34" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="34" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="H12" s="34" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="I12" s="35" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
@@ -3456,19 +4427,19 @@
         <v>24</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>152</v>
-      </c>
-      <c r="F13" s="45" t="s">
-        <v>181</v>
+        <v>136</v>
+      </c>
+      <c r="F13" s="43" t="s">
+        <v>165</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="H13" s="34" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="I13" s="35"/>
     </row>
@@ -3480,19 +4451,19 @@
         <v>24</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>152</v>
-      </c>
-      <c r="F14" s="45" t="s">
-        <v>181</v>
+        <v>136</v>
+      </c>
+      <c r="F14" s="43" t="s">
+        <v>165</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="H14" s="34" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="I14" s="35"/>
     </row>
@@ -3504,19 +4475,19 @@
         <v>24</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F15" s="45" t="s">
-        <v>181</v>
+        <v>146</v>
+      </c>
+      <c r="F15" s="43" t="s">
+        <v>165</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="H15" s="34" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
@@ -3527,19 +4498,19 @@
         <v>24</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="F16" s="45" t="s">
-        <v>181</v>
+        <v>147</v>
+      </c>
+      <c r="F16" s="43" t="s">
+        <v>165</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
@@ -3550,19 +4521,19 @@
         <v>24</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="F17" s="45" t="s">
-        <v>181</v>
+        <v>153</v>
+      </c>
+      <c r="F17" s="43" t="s">
+        <v>165</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="H17" s="34" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
@@ -3573,19 +4544,19 @@
         <v>24</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="F18" s="39" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="G18" s="39" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="H18" s="39" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="I18" s="42"/>
     </row>
@@ -3593,389 +4564,369 @@
       <c r="B19" s="3">
         <v>15</v>
       </c>
-      <c r="C19" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="D19" s="44" t="s">
-        <v>173</v>
-      </c>
-      <c r="E19" s="44" t="s">
+      <c r="C19" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="E19" s="34" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="34" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="G19" s="34" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
         <v>16</v>
       </c>
-      <c r="C20" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="D20" s="44" t="s">
-        <v>174</v>
-      </c>
-      <c r="E20" s="44" t="s">
+      <c r="C20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="E20" s="34" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="3">
         <v>17</v>
       </c>
-      <c r="C21" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="D21" s="44" t="s">
-        <v>175</v>
-      </c>
-      <c r="E21" s="44" t="s">
+      <c r="C21" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="E21" s="34" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="3">
         <v>18</v>
       </c>
-      <c r="C22" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="D22" s="44" t="s">
-        <v>176</v>
-      </c>
-      <c r="E22" s="44" t="s">
-        <v>183</v>
+      <c r="C22" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="E22" s="34" t="s">
+        <v>167</v>
       </c>
       <c r="F22" s="34" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="I22" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="3">
         <v>19</v>
       </c>
-      <c r="C23" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="D23" s="44" t="s">
-        <v>177</v>
-      </c>
-      <c r="E23" s="44" t="s">
-        <v>184</v>
+      <c r="C23" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>168</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="G23" s="34" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="I23" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="3">
         <v>20</v>
       </c>
-      <c r="C24" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="D24" s="44" t="s">
-        <v>178</v>
-      </c>
-      <c r="E24" s="44" t="s">
-        <v>185</v>
+      <c r="C24" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>169</v>
       </c>
       <c r="F24" s="34" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="G24" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="38">
         <v>21</v>
       </c>
-      <c r="C25" s="46" t="s">
-        <v>115</v>
-      </c>
-      <c r="D25" s="47" t="s">
+      <c r="C25" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="E25" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="F25" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="G25" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="H25" s="39" t="s">
+        <v>170</v>
+      </c>
+      <c r="I25" s="42"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="3">
+        <v>22</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="E26" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="H26" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="3">
+        <v>23</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="E27" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="G27" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="H27" s="34" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" s="3">
+        <v>24</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="G28" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="H28" s="35" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" s="3">
+        <v>25</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="E29" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="F29" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="G29" s="34" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" s="3">
+        <v>26</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="F30" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="G30" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="38">
+        <v>27</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="E25" s="47" t="s">
-        <v>169</v>
-      </c>
-      <c r="F25" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="G25" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="H25" s="39" t="s">
-        <v>186</v>
-      </c>
-      <c r="I25" s="42"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B26" s="43">
-        <v>22</v>
-      </c>
-      <c r="C26" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="44" t="s">
-        <v>187</v>
-      </c>
-      <c r="E26" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="G26" s="44" t="s">
-        <v>157</v>
-      </c>
-      <c r="H26" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B27" s="43">
-        <v>23</v>
-      </c>
-      <c r="C27" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="44" t="s">
-        <v>189</v>
-      </c>
-      <c r="E27" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="G27" s="44" t="s">
-        <v>157</v>
-      </c>
-      <c r="H27" s="44" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B28" s="43">
-        <v>24</v>
-      </c>
-      <c r="C28" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="44" t="s">
-        <v>190</v>
-      </c>
-      <c r="E28" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="G28" s="44" t="s">
-        <v>157</v>
-      </c>
-      <c r="H28" s="48" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B29" s="43">
-        <v>25</v>
-      </c>
-      <c r="C29" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="E29" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="F29" s="44" t="s">
-        <v>180</v>
-      </c>
-      <c r="G29" s="44" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B30" s="43">
-        <v>26</v>
-      </c>
-      <c r="C30" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="44" t="s">
-        <v>198</v>
-      </c>
-      <c r="E30" s="44" t="s">
-        <v>184</v>
-      </c>
-      <c r="F30" s="44" t="s">
-        <v>181</v>
-      </c>
-      <c r="G30" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B31" s="46">
-        <v>27</v>
-      </c>
-      <c r="C31" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="E31" s="47" t="s">
-        <v>169</v>
-      </c>
-      <c r="F31" s="47" t="s">
-        <v>181</v>
-      </c>
-      <c r="G31" s="47" t="s">
-        <v>170</v>
+      <c r="E31" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="F31" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="G31" s="39" t="s">
+        <v>154</v>
       </c>
       <c r="H31" s="42"/>
       <c r="I31" s="42"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B32" s="43">
+      <c r="B32" s="3">
         <v>28</v>
       </c>
-      <c r="C32" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="D32" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="E32" s="44" t="s">
+      <c r="C32" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E32" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F32" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="G32" s="44" t="s">
-        <v>157</v>
+      <c r="F32" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="G32" s="34" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="43">
+      <c r="B33" s="3">
         <v>29</v>
       </c>
-      <c r="C33" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="D33" s="44" t="s">
-        <v>197</v>
-      </c>
-      <c r="E33" s="44" t="s">
+      <c r="C33" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="E33" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F33" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="G33" s="44" t="s">
-        <v>157</v>
+      <c r="F33" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="G33" s="34" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="43">
+      <c r="B34" s="3">
         <v>30</v>
       </c>
-      <c r="C34" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="D34" s="44" t="s">
-        <v>200</v>
-      </c>
-      <c r="E34" s="44" t="s">
+      <c r="C34" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="E34" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F34" s="44" t="s">
-        <v>201</v>
-      </c>
-      <c r="G34" s="44" t="s">
-        <v>157</v>
+      <c r="F34" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="G34" s="34" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B35" s="43">
+      <c r="B35" s="38">
         <v>31</v>
       </c>
-      <c r="C35" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="D35" s="44" t="s">
-        <v>199</v>
-      </c>
-      <c r="E35" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="G35" s="34" t="s">
-        <v>158</v>
-      </c>
+      <c r="C35" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="E35" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="F35" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="G35" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="H35" s="42"/>
+      <c r="I35" s="42"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B36" s="46">
-        <v>32</v>
-      </c>
-      <c r="C36" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="D36" s="47" t="s">
-        <v>194</v>
-      </c>
-      <c r="E36" s="47" t="s">
-        <v>184</v>
-      </c>
-      <c r="F36" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="G36" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="H36" s="42"/>
-      <c r="I36" s="42"/>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="44"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update Sample Data.xlsx, add Cars route and make seed.py work
</commit_message>
<xml_diff>
--- a/assets/Project Sample Data.xlsx
+++ b/assets/Project Sample Data.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/student/Desktop/Phase-5-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/student/Development/code/Phase-5-Project/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E687D5-F34E-FD4F-A525-9C47C4B38010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD92412-EEDF-D043-8ACA-2D2D9FB86598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="5080" windowWidth="28740" windowHeight="14660" activeTab="5" xr2:uid="{32EFB3F7-074C-4947-9292-1B2AC616E0B4}"/>
+    <workbookView xWindow="800" yWindow="5080" windowWidth="19840" windowHeight="14660" activeTab="4" xr2:uid="{32EFB3F7-074C-4947-9292-1B2AC616E0B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="User" sheetId="3" r:id="rId2"/>
     <sheet name="Location" sheetId="6" r:id="rId3"/>
     <sheet name="House" sheetId="4" r:id="rId4"/>
-    <sheet name="Flight" sheetId="5" r:id="rId5"/>
-    <sheet name="Aircraft" sheetId="8" r:id="rId6"/>
-    <sheet name="Variables" sheetId="7" r:id="rId7"/>
+    <sheet name="Car" sheetId="9" r:id="rId5"/>
+    <sheet name="Flight" sheetId="5" r:id="rId6"/>
+    <sheet name="Aircraft" sheetId="8" r:id="rId7"/>
+    <sheet name="Variables" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="252">
   <si>
     <t>User</t>
   </si>
@@ -879,6 +880,69 @@
   </si>
   <si>
     <t>CO2 per Trip and pass</t>
+  </si>
+  <si>
+    <t>Model: Car</t>
+  </si>
+  <si>
+    <t>Make</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Miles per Year</t>
+  </si>
+  <si>
+    <t>mpg</t>
+  </si>
+  <si>
+    <t>CO2 Produced</t>
+  </si>
+  <si>
+    <t>location_id</t>
+  </si>
+  <si>
+    <t>Honda</t>
+  </si>
+  <si>
+    <t>Accord</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>actual</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>Explorer</t>
+  </si>
+  <si>
+    <t>Chevrolet</t>
+  </si>
+  <si>
+    <t>Malibu</t>
+  </si>
+  <si>
+    <t>Mustang</t>
+  </si>
+  <si>
+    <t>Volkswagen</t>
+  </si>
+  <si>
+    <t>Silverado</t>
+  </si>
+  <si>
+    <t>Civic</t>
+  </si>
+  <si>
+    <t>Tiguan</t>
+  </si>
+  <si>
+    <t>kg/ Year</t>
   </si>
 </sst>
 </file>
@@ -1010,7 +1074,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1127,22 +1191,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1153,6 +1201,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1169,6 +1220,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>18012</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E830D31-E5C7-5092-C3A7-83411665C1D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="711200" y="4622800"/>
+          <a:ext cx="7772400" cy="4386812"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>116876</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{807EEF37-E3E0-2617-6ECD-8D217396BB4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9410700" y="4584700"/>
+          <a:ext cx="7772400" cy="5336576"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1947,7 +2091,7 @@
   <dimension ref="B2:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2875,6 +3019,439 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD15C7A-8629-1D4D-9CD6-994AE81A3015}">
+  <dimension ref="B2:J18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="13.83203125" style="2" customWidth="1"/>
+    <col min="4" max="8" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H3" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2018</v>
+      </c>
+      <c r="F5" s="3">
+        <v>17396</v>
+      </c>
+      <c r="G5" s="3">
+        <v>30</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1188</v>
+      </c>
+      <c r="I5" s="48">
+        <f>8.89/G5*F5</f>
+        <v>5155.0146666666669</v>
+      </c>
+      <c r="J5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2024</v>
+      </c>
+      <c r="F6" s="3">
+        <v>15196</v>
+      </c>
+      <c r="G6" s="3">
+        <v>22</v>
+      </c>
+      <c r="H6" s="3">
+        <v>991</v>
+      </c>
+      <c r="I6" s="48">
+        <f t="shared" ref="I6:I14" si="0">8.89/G6*F6</f>
+        <v>6140.5654545454545</v>
+      </c>
+      <c r="J6" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="3">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2016</v>
+      </c>
+      <c r="F7" s="3">
+        <v>15653</v>
+      </c>
+      <c r="G7" s="3">
+        <v>30</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1461</v>
+      </c>
+      <c r="I7" s="48">
+        <f t="shared" si="0"/>
+        <v>4638.5056666666669</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="3">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2018</v>
+      </c>
+      <c r="F8" s="3">
+        <v>18036</v>
+      </c>
+      <c r="G8" s="3">
+        <v>29</v>
+      </c>
+      <c r="H8" s="3">
+        <v>762</v>
+      </c>
+      <c r="I8" s="48">
+        <f t="shared" si="0"/>
+        <v>5528.9668965517249</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="3">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2016</v>
+      </c>
+      <c r="F9" s="3">
+        <v>19237</v>
+      </c>
+      <c r="G9" s="3">
+        <v>25</v>
+      </c>
+      <c r="H9" s="3">
+        <v>698</v>
+      </c>
+      <c r="I9" s="48">
+        <f t="shared" si="0"/>
+        <v>6840.6772000000001</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="3">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2024</v>
+      </c>
+      <c r="F10" s="3">
+        <v>9178</v>
+      </c>
+      <c r="G10" s="3">
+        <v>21</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1464</v>
+      </c>
+      <c r="I10" s="48">
+        <f t="shared" si="0"/>
+        <v>3885.3533333333335</v>
+      </c>
+      <c r="J10" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="3">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E11" s="3">
+        <v>2015</v>
+      </c>
+      <c r="F11" s="3">
+        <v>10944</v>
+      </c>
+      <c r="G11" s="3">
+        <v>33</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1708</v>
+      </c>
+      <c r="I11" s="48">
+        <f t="shared" si="0"/>
+        <v>2948.247272727273</v>
+      </c>
+      <c r="J11" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="3">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2023</v>
+      </c>
+      <c r="F12" s="3">
+        <v>13005</v>
+      </c>
+      <c r="G12" s="3">
+        <v>30</v>
+      </c>
+      <c r="H12" s="3">
+        <v>681</v>
+      </c>
+      <c r="I12" s="48">
+        <f t="shared" si="0"/>
+        <v>3853.8150000000001</v>
+      </c>
+      <c r="J12" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="3">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E13" s="3">
+        <v>2005</v>
+      </c>
+      <c r="F13" s="3">
+        <v>9245</v>
+      </c>
+      <c r="G13" s="3">
+        <v>29</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1609</v>
+      </c>
+      <c r="I13" s="48">
+        <f t="shared" si="0"/>
+        <v>2834.0706896551728</v>
+      </c>
+      <c r="J13" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="3">
+        <v>10</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="E14" s="3">
+        <v>2007</v>
+      </c>
+      <c r="F14" s="3">
+        <v>15376</v>
+      </c>
+      <c r="G14" s="3">
+        <v>24</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1042</v>
+      </c>
+      <c r="I14" s="48">
+        <f t="shared" si="0"/>
+        <v>5695.5266666666666</v>
+      </c>
+      <c r="J14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3">
+        <f>MIN(F5:F14)</f>
+        <v>9178</v>
+      </c>
+      <c r="G16" s="3">
+        <f>MIN(G5:G14)</f>
+        <v>21</v>
+      </c>
+      <c r="H16" s="3">
+        <f>MIN(H5:H14)</f>
+        <v>681</v>
+      </c>
+      <c r="I16" s="48">
+        <f>MIN(I5:I14)</f>
+        <v>2834.0706896551728</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="3">
+        <f>AVERAGE(F5:F14)</f>
+        <v>14326.6</v>
+      </c>
+      <c r="G17" s="3">
+        <f>AVERAGE(G5:G14)</f>
+        <v>27.3</v>
+      </c>
+      <c r="H17" s="3">
+        <f>AVERAGE(H5:H14)</f>
+        <v>1160.4000000000001</v>
+      </c>
+      <c r="I17" s="48">
+        <f>AVERAGE(I5:I14)</f>
+        <v>4752.0742846812955</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="3">
+        <f>MAX(F5:F14)</f>
+        <v>19237</v>
+      </c>
+      <c r="G18" s="3">
+        <f>MAX(G5:G14)</f>
+        <v>33</v>
+      </c>
+      <c r="H18" s="3">
+        <f>MAX(H5:H14)</f>
+        <v>1708</v>
+      </c>
+      <c r="I18" s="48">
+        <f>MAX(I5:I14)</f>
+        <v>6840.6772000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1250A8-6E80-0C46-A8F8-0559EC6AFD80}">
   <dimension ref="B2:U50"/>
   <sheetViews>
@@ -2930,7 +3507,7 @@
       <c r="H3" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="I3" s="54" t="s">
+      <c r="I3" s="46" t="s">
         <v>207</v>
       </c>
       <c r="J3" s="22" t="s">
@@ -2959,7 +3536,7 @@
       <c r="H4" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="I4" s="52" t="s">
+      <c r="I4" s="44" t="s">
         <v>60</v>
       </c>
       <c r="J4" s="23" t="s">
@@ -3001,7 +3578,7 @@
       <c r="H5" s="19">
         <v>2414</v>
       </c>
-      <c r="I5" s="53">
+      <c r="I5" s="45">
         <v>0.35</v>
       </c>
       <c r="J5" s="24">
@@ -3034,7 +3611,7 @@
       <c r="H6" s="19">
         <v>7494</v>
       </c>
-      <c r="I6" s="53">
+      <c r="I6" s="45">
         <v>0.25</v>
       </c>
       <c r="J6" s="24">
@@ -3067,7 +3644,7 @@
       <c r="H7" s="19">
         <v>3942</v>
       </c>
-      <c r="I7" s="53">
+      <c r="I7" s="45">
         <v>0.4</v>
       </c>
       <c r="J7" s="24">
@@ -3100,7 +3677,7 @@
       <c r="H8" s="19">
         <v>1075</v>
       </c>
-      <c r="I8" s="53">
+      <c r="I8" s="45">
         <v>0.3</v>
       </c>
       <c r="J8" s="24">
@@ -3115,233 +3692,142 @@
       <c r="B9" s="3">
         <v>5</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="44"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>6</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="44"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <v>7</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="44"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <v>8</v>
       </c>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="44"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <v>9</v>
       </c>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="44"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
         <v>10</v>
       </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="44"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <v>11</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <v>12</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="44"/>
-      <c r="L16" s="44"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="3">
         <v>13</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="44"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="3">
         <v>14</v>
       </c>
-      <c r="C18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="44"/>
-      <c r="L18" s="48"/>
+      <c r="L18" s="9"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <v>15</v>
       </c>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="49"/>
+      <c r="L19" s="6"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
         <v>16</v>
       </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="49"/>
+      <c r="L20" s="6"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="3">
         <v>17</v>
       </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="49"/>
+      <c r="L21" s="6"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="3">
         <v>18</v>
       </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="49"/>
+      <c r="L22" s="6"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="3">
         <v>19</v>
       </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="49"/>
+      <c r="L23" s="6"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="3">
         <v>20</v>
       </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="49"/>
+      <c r="L24" s="6"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="L25" s="6"/>
@@ -3504,11 +3990,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247AF918-C098-5746-A618-04E4B77230F3}">
-  <dimension ref="B1:U50"/>
+  <dimension ref="B2:U50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -3536,81 +4022,61 @@
     <col min="22" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-    </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="44"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C3" s="44"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44" t="s">
+      <c r="D3" s="1"/>
+      <c r="G3" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="H4" s="46" t="s">
+      <c r="H4" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="I4" s="46" t="s">
+      <c r="I4" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="J4" s="46" t="s">
+      <c r="J4" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="K4" s="46" t="s">
+      <c r="K4" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="L4" s="45"/>
+      <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -3625,10 +4091,10 @@
       <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="D5" s="47" t="b">
+      <c r="D5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E5" s="2">
@@ -3649,23 +4115,22 @@
         <f>H5/E5/G5*1000</f>
         <v>44.444444444444436</v>
       </c>
-      <c r="J5" s="47">
+      <c r="J5" s="3">
         <v>90</v>
       </c>
-      <c r="K5" s="47">
+      <c r="K5" s="3">
         <f>H5/E5</f>
         <v>217.25999999999996</v>
       </c>
-      <c r="L5" s="44"/>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
         <v>2</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="D6" s="47" t="b">
+      <c r="D6" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E6" s="2">
@@ -3686,23 +4151,22 @@
         <f>H6/E6/G6*1000</f>
         <v>27.027027027027028</v>
       </c>
-      <c r="J6" s="47">
+      <c r="J6" s="3">
         <v>100</v>
       </c>
-      <c r="K6" s="47">
+      <c r="K6" s="3">
         <f>H6/E6</f>
         <v>824.34000000000015</v>
       </c>
-      <c r="L6" s="44"/>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B7" s="3">
         <v>3</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D7" s="47" t="b">
+      <c r="D7" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2">
@@ -3723,23 +4187,22 @@
         <f>H7/E7/G7*1000</f>
         <v>45.454545454545453</v>
       </c>
-      <c r="J7" s="47">
+      <c r="J7" s="3">
         <v>80</v>
       </c>
-      <c r="K7" s="47">
+      <c r="K7" s="3">
         <f>H7/E7</f>
         <v>354.78000000000003</v>
       </c>
-      <c r="L7" s="44"/>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B8" s="3">
         <v>4</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="D8" s="47" t="b">
+      <c r="D8" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E8" s="2">
@@ -3760,303 +4223,158 @@
         <f>H8/E8/G8*1000</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="J8" s="47">
+      <c r="J8" s="3">
         <v>80</v>
       </c>
-      <c r="K8" s="47">
+      <c r="K8" s="3">
         <f>H8/E8</f>
         <v>75.25</v>
       </c>
-      <c r="L8" s="44"/>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B9" s="3">
         <v>5</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="44"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="44"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="44"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B12" s="3"/>
-      <c r="C12" s="47"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="44"/>
+      <c r="C12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B13" s="3"/>
-      <c r="C13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="44"/>
+      <c r="C13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
-      <c r="C14" s="47"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="44"/>
+      <c r="C14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="44"/>
-      <c r="L16" s="44"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="47" t="s">
         <v>213</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="44"/>
+      <c r="C17" s="3"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="55" t="s">
+      <c r="B18" s="47" t="s">
         <v>214</v>
       </c>
-      <c r="C18" s="47"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="44"/>
-      <c r="L18" s="48"/>
+      <c r="C18" s="3"/>
+      <c r="L18" s="9"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="47" t="s">
         <v>215</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="49"/>
+      <c r="C19" s="3"/>
+      <c r="L19" s="6"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="47" t="s">
         <v>216</v>
       </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="49"/>
+      <c r="L20" s="6"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="49"/>
+      <c r="L21" s="6"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="47" t="s">
         <v>217</v>
       </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="49"/>
+      <c r="L22" s="6"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B23" s="55" t="s">
+      <c r="B23" s="47" t="s">
         <v>218</v>
       </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="49"/>
+      <c r="L23" s="6"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B24" s="55" t="s">
+      <c r="B24" s="47" t="s">
         <v>219</v>
       </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="49"/>
+      <c r="L24" s="6"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B25" s="55" t="s">
+      <c r="B25" s="47" t="s">
         <v>220</v>
       </c>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="44"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="49"/>
+      <c r="L25" s="6"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="44"/>
-      <c r="K26" s="44"/>
-      <c r="L26" s="49"/>
+      <c r="L26" s="6"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="47" t="s">
         <v>221</v>
       </c>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="49"/>
+      <c r="L27" s="6"/>
     </row>
     <row r="28" spans="2:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="B28" s="55" t="s">
+      <c r="B28" s="47" t="s">
         <v>222</v>
       </c>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="50"/>
+      <c r="L28" s="7"/>
     </row>
     <row r="29" spans="2:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="B29" s="55" t="s">
+      <c r="B29" s="47" t="s">
         <v>223</v>
       </c>
-      <c r="C29" s="50"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="44"/>
+      <c r="C29" s="7"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B30" s="55" t="s">
+      <c r="B30" s="47" t="s">
         <v>224</v>
       </c>
-      <c r="C30" s="51"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="44"/>
-      <c r="L30" s="44"/>
+      <c r="C30" s="25"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C31" s="25"/>
@@ -4157,7 +4475,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47C0C0F9-708C-F34C-ABB4-7A88469AE5BB}">
   <dimension ref="B2:I36"/>
   <sheetViews>

</xml_diff>

<commit_message>
add API Routes for User and House
</commit_message>
<xml_diff>
--- a/assets/Project Sample Data.xlsx
+++ b/assets/Project Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/student/Development/code/Phase-5-Project/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD92412-EEDF-D043-8ACA-2D2D9FB86598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCEBD94-D01E-9640-AF01-126E6A5560B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="5080" windowWidth="19840" windowHeight="14660" activeTab="4" xr2:uid="{32EFB3F7-074C-4947-9292-1B2AC616E0B4}"/>
+    <workbookView xWindow="800" yWindow="5080" windowWidth="19840" windowHeight="14660" activeTab="3" xr2:uid="{32EFB3F7-074C-4947-9292-1B2AC616E0B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -2425,8 +2425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE410F25-C2D1-0E47-B65D-2476561BC1C2}">
   <dimension ref="B2:L21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="125" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3022,7 +3022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD15C7A-8629-1D4D-9CD6-994AE81A3015}">
   <dimension ref="B2:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add flights into User API Route in app.py - now accumulates CO2 for all flights for each user
</commit_message>
<xml_diff>
--- a/assets/Project Sample Data.xlsx
+++ b/assets/Project Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/student/Development/code/Phase-5-Project/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCEBD94-D01E-9640-AF01-126E6A5560B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB9F92D-B7EA-444B-99EC-1735D8F56C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="5080" windowWidth="19840" windowHeight="14660" activeTab="3" xr2:uid="{32EFB3F7-074C-4947-9292-1B2AC616E0B4}"/>
+    <workbookView xWindow="620" yWindow="9680" windowWidth="19840" windowHeight="14660" activeTab="4" xr2:uid="{32EFB3F7-074C-4947-9292-1B2AC616E0B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -2425,8 +2425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE410F25-C2D1-0E47-B65D-2476561BC1C2}">
   <dimension ref="B2:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView topLeftCell="E2" zoomScale="125" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3022,8 +3022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD15C7A-8629-1D4D-9CD6-994AE81A3015}">
   <dimension ref="B2:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>